<commit_message>
Adjusted angles in cpl file.
</commit_message>
<xml_diff>
--- a/hardware/pcbs/multiplexer_v0p3/gerber_v0p3/fab_files/CPL_JLCPCB.xlsx
+++ b/hardware/pcbs/multiplexer_v0p3/gerber_v0p3/fab_files/CPL_JLCPCB.xlsx
@@ -222,7 +222,7 @@
   <dimension ref="A1:E1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="E27" activeCellId="0" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -472,7 +472,7 @@
         <v>6</v>
       </c>
       <c r="E14" s="2" t="n">
-        <v>0</v>
+        <v>-90</v>
       </c>
     </row>
     <row r="15" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -489,7 +489,7 @@
         <v>6</v>
       </c>
       <c r="E15" s="2" t="n">
-        <v>0</v>
+        <v>-90</v>
       </c>
     </row>
     <row r="16" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -506,7 +506,7 @@
         <v>6</v>
       </c>
       <c r="E16" s="2" t="n">
-        <v>0</v>
+        <v>-90</v>
       </c>
     </row>
     <row r="17" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -523,117 +523,9 @@
         <v>6</v>
       </c>
       <c r="E17" s="2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="1048451" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048452" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048453" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048454" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048455" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048456" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048457" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048458" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048459" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048460" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048461" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048462" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048463" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048464" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048465" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048466" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048467" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048468" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048469" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048470" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048471" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048472" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048473" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048474" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048475" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048476" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048477" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048478" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048479" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048480" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048481" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048482" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048483" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048484" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048485" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048486" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048487" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048488" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048489" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048490" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048491" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048492" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048493" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048494" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048495" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048496" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048497" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048498" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048499" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048500" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048501" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048502" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048503" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048504" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048505" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048506" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048507" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048508" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048509" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048510" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048511" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048512" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048513" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048514" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048515" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048516" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048517" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048518" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048519" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048520" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048521" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048522" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048523" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048524" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048525" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048526" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048527" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048528" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048529" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048530" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048531" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048532" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048533" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048534" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048535" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048536" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048537" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048538" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048539" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048540" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048541" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048542" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048543" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048544" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048545" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048546" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048547" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048548" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048549" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048550" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048551" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048552" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048553" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048554" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048555" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048556" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048557" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048558" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+        <v>-90</v>
+      </c>
+    </row>
     <row r="1048559" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048560" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048561" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>